<commit_message>
Update API URL with current ngrok endpoint
</commit_message>
<xml_diff>
--- a/FP.xlsx
+++ b/FP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1amsh\Desktop\ExcelApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6A009F-7D4E-43CA-A607-740515569D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C842B1-7E45-49E6-9994-DB6DB25F0416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4176" yWindow="3720" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MBA_year" sheetId="1" r:id="rId1"/>

</xml_diff>